<commit_message>
Ajuste Final de Atualizacao de Cenarios de Teste
</commit_message>
<xml_diff>
--- a/CenariosDeTeste_Grupo6.xlsx
+++ b/CenariosDeTeste_Grupo6.xlsx
@@ -87,10 +87,10 @@
 Senha para login: admin123
 User Role: Admin
 Status: Enabled
-Employee Name: Lisa Andrews
-Username: grupo_6_teste
-Password: teste1234
-Confirm Password: teste1234</t>
+Employee Name: Qualquer um que tenha a letra A
+Username: Nome Usuario + numero aleatorio(1 a 999)
+Password:Abcd@1234
+Confirm Password: Abcd@1234</t>
   </si>
   <si>
     <t xml:space="preserve">Ambiente </t>
@@ -122,7 +122,7 @@
   <si>
     <t>Nome de usuário para login: Admin
 Senha para login: admin123
-Username: grupo_6_teste</t>
+Username: Nome do usuario cadastrado previamente</t>
   </si>
   <si>
     <t>Caso de Teste CT-003 - Editar usuário</t>
@@ -146,8 +146,8 @@
   <si>
     <t>Nome de usuário para login: Admin
 Senha para login: admin123
-[Antigo]Username: grupo_6_teste
-[Novo]Username: grupo_6_teste_sistema</t>
+[Antigo]Username: Nome do usuário cadastrado previamente
+[Novo]Username: Nome do novo usuario gerado</t>
   </si>
   <si>
     <t>Caso de Teste CT-004 - Ordenar usuários</t>
@@ -155,14 +155,14 @@
   <si>
     <t>1 - Acessar menu [Admin]
 2 - Clicar no ícone seta da coluna Employee Name
-3 - Selecionar a opção Ascending
+3 - Selecionar a opção Ascending pelo nome do usuario
 4 - Verificar a ordenação dos registros dos usuários</t>
   </si>
   <si>
     <t>1 - Tela de gerenciamento de usuários/admin deve ser exibida
 2 - Lista de opções de ordenação deve ser exibida
 3 - 
-4 - Registro de usuários deve ser ordenado na ordem alfábetica do Employee Name</t>
+4 - Registro de usuários deve ser ordenado na ordem alfábetica do Nome do usuario</t>
   </si>
   <si>
     <t>Nome de usuário para login: Admin
@@ -185,7 +185,9 @@
   <si>
     <t>Nome de usuário para login: Admin
 Senha para login: admin123
-User Role: ESS</t>
+Username: Nome do usuario cadastrado previamente
+User Role: ESS
+Status: Admin</t>
   </si>
   <si>
     <t>Caso de Teste CT-006 - Resetar pesquisa de usuário</t>
@@ -203,9 +205,9 @@
   <si>
     <t>Nome de usuário para login: Admin
 Senha para login: admin123
-Username: admin
-User Role: Admin
-Status: Enablead</t>
+Username: Admin
+User Role: ESS
+Status: Disabled</t>
   </si>
   <si>
     <t>Caso de Teste CT-007 - Comentar em um post no menu Buzz</t>
@@ -1799,7 +1801,7 @@
       <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2867,7 +2869,7 @@
       <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3935,7 +3937,7 @@
       <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>